<commit_message>
Moved parsing of master classification and model config file to new functions defined in ODYM.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_0.xlsx
+++ b/RECC_Config_V2_0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9405" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -1727,9 +1727,6 @@
     <t>RECC_Classifications_Master_V2.0</t>
   </si>
   <si>
-    <t>RECC_Germany</t>
-  </si>
-  <si>
     <t>Region32</t>
   </si>
   <si>
@@ -2127,6 +2124,9 @@
   </si>
   <si>
     <t>[12]</t>
+  </si>
+  <si>
+    <t>RECC_G7</t>
   </si>
 </sst>
 </file>
@@ -2859,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2900,7 +2900,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="81" t="s">
-        <v>567</v>
+        <v>700</v>
       </c>
       <c r="G4" s="28"/>
     </row>
@@ -6279,7 +6279,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -6490,7 +6490,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C21" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D21" s="69" t="s">
         <v>55</v>
@@ -6502,7 +6502,7 @@
         <v>56</v>
       </c>
       <c r="G21" s="69" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H21" s="70" t="s">
         <v>58</v>
@@ -6513,7 +6513,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C22" s="68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D22" s="69" t="s">
         <v>55</v>
@@ -6522,21 +6522,21 @@
         <v>54</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H22" s="70" t="s">
+        <v>576</v>
+      </c>
+      <c r="I22" s="69" t="s">
         <v>577</v>
-      </c>
-      <c r="I22" s="69" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C23" s="68" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D23" s="69" t="s">
         <v>55</v>
@@ -6545,22 +6545,22 @@
         <v>54</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="70" t="s">
+        <v>574</v>
+      </c>
+      <c r="I23" s="69" t="s">
         <v>575</v>
-      </c>
-      <c r="I23" s="69" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="59"/>
       <c r="C24" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>55</v>
@@ -6569,16 +6569,16 @@
         <v>54</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G24" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H24" s="70" t="s">
+        <v>614</v>
+      </c>
+      <c r="I24" s="69" t="s">
         <v>615</v>
-      </c>
-      <c r="I24" s="69" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -6652,19 +6652,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C28" s="68" t="s">
+        <v>579</v>
+      </c>
+      <c r="D28" s="69" t="s">
         <v>580</v>
       </c>
-      <c r="D28" s="69" t="s">
-        <v>581</v>
-      </c>
       <c r="E28" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H28" s="70" t="s">
         <v>140</v>
@@ -6678,10 +6678,10 @@
         <v>91</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E29" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F29" s="69" t="s">
         <v>93</v>
@@ -6698,22 +6698,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C30" s="68" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E30" s="69" t="s">
+        <v>596</v>
+      </c>
+      <c r="F30" s="69" t="s">
         <v>597</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>598</v>
       </c>
       <c r="G30" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H30" s="70" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I30" s="69" t="s">
         <v>501</v>
@@ -6721,140 +6721,140 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C31" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="D31" s="69" t="s">
         <v>590</v>
       </c>
-      <c r="D31" s="69" t="s">
-        <v>591</v>
-      </c>
       <c r="E31" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C32" s="68" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H32" s="70" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C33" s="68" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F33" s="69" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G33" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H33" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="I33" s="69" t="s">
         <v>610</v>
-      </c>
-      <c r="I33" s="69" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C34" s="68" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E34" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G34" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H34" s="70" t="s">
+        <v>616</v>
+      </c>
+      <c r="I34" s="69" t="s">
         <v>617</v>
-      </c>
-      <c r="I34" s="69" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C35" s="68" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E35" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G35" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H35" s="70" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I35" s="69" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C36" s="68" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D36" s="69" t="s">
+        <v>595</v>
+      </c>
+      <c r="E36" s="69" t="s">
         <v>596</v>
       </c>
-      <c r="E36" s="69" t="s">
-        <v>597</v>
-      </c>
       <c r="F36" s="69" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G36" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H36" s="70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.45">
@@ -7049,7 +7049,7 @@
         <v>148</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45" s="69" t="s">
         <v>149</v>
@@ -7387,7 +7387,7 @@
         <v>194</v>
       </c>
       <c r="E71" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F71" s="73" t="s">
         <v>196</v>
@@ -7426,16 +7426,16 @@
         <v>167</v>
       </c>
       <c r="C72" s="82" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D72" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E72" s="69" t="s">
+        <v>620</v>
+      </c>
+      <c r="F72" s="73" t="s">
         <v>621</v>
-      </c>
-      <c r="F72" s="73" t="s">
-        <v>622</v>
       </c>
       <c r="G72" s="69" t="s">
         <v>197</v>
@@ -7444,7 +7444,7 @@
         <v>134</v>
       </c>
       <c r="I72" s="41" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J72" s="41" t="s">
         <v>209</v>
@@ -7471,16 +7471,16 @@
         <v>167</v>
       </c>
       <c r="C73" s="82" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D73" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E73" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F73" s="73" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G73" s="69" t="s">
         <v>197</v>
@@ -7489,7 +7489,7 @@
         <v>134</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J73" s="41" t="s">
         <v>209</v>
@@ -7516,13 +7516,13 @@
         <v>167</v>
       </c>
       <c r="C74" s="82" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D74" s="69" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E74" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F74" s="73" t="s">
         <v>217</v>
@@ -7534,7 +7534,7 @@
         <v>134</v>
       </c>
       <c r="I74" s="63" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J74" s="41" t="s">
         <v>199</v>
@@ -7561,13 +7561,13 @@
         <v>167</v>
       </c>
       <c r="C75" s="82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D75" s="69" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E75" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F75" s="73" t="s">
         <v>217</v>
@@ -7579,7 +7579,7 @@
         <v>134</v>
       </c>
       <c r="I75" s="63" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J75" s="41" t="s">
         <v>199</v>
@@ -7606,16 +7606,16 @@
         <v>167</v>
       </c>
       <c r="C76" s="84" t="s">
+        <v>632</v>
+      </c>
+      <c r="D76" s="85" t="s">
         <v>633</v>
       </c>
-      <c r="D76" s="85" t="s">
-        <v>634</v>
-      </c>
       <c r="E76" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G76" s="74" t="s">
         <v>227</v>
@@ -7624,7 +7624,7 @@
         <v>134</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J76" s="40" t="s">
         <v>199</v>
@@ -7651,16 +7651,16 @@
         <v>167</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D77" s="85" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E77" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F77" s="77" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G77" s="74" t="s">
         <v>227</v>
@@ -7669,7 +7669,7 @@
         <v>134</v>
       </c>
       <c r="I77" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J77" s="40" t="s">
         <v>199</v>
@@ -7702,7 +7702,7 @@
         <v>233</v>
       </c>
       <c r="E78" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F78" s="75" t="s">
         <v>235</v>
@@ -7747,10 +7747,10 @@
         <v>240</v>
       </c>
       <c r="E79" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F79" s="73" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G79" s="69" t="s">
         <v>243</v>
@@ -7786,16 +7786,16 @@
         <v>167</v>
       </c>
       <c r="C80" s="84" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D80" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E80" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F80" s="73" t="s">
         <v>645</v>
-      </c>
-      <c r="F80" s="73" t="s">
-        <v>646</v>
       </c>
       <c r="G80" s="69" t="s">
         <v>129</v>
@@ -7831,16 +7831,16 @@
         <v>167</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D81" s="69" t="s">
+        <v>643</v>
+      </c>
+      <c r="E81" s="69" t="s">
         <v>644</v>
       </c>
-      <c r="E81" s="69" t="s">
-        <v>645</v>
-      </c>
       <c r="F81" s="73" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G81" s="69" t="s">
         <v>129</v>
@@ -7849,7 +7849,7 @@
         <v>134</v>
       </c>
       <c r="I81" s="41" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J81" s="41" t="s">
         <v>209</v>
@@ -7882,10 +7882,10 @@
         <v>256</v>
       </c>
       <c r="E82" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F82" s="77" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G82" s="85" t="s">
         <v>197</v>
@@ -7927,10 +7927,10 @@
         <v>263</v>
       </c>
       <c r="E83" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F83" s="77" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G83" s="85" t="s">
         <v>197</v>
@@ -7972,7 +7972,7 @@
         <v>268</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F84" s="73" t="s">
         <v>270</v>
@@ -8017,7 +8017,7 @@
         <v>277</v>
       </c>
       <c r="E85" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F85" s="73" t="s">
         <v>270</v>
@@ -8064,7 +8064,7 @@
         <v>282</v>
       </c>
       <c r="E86" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F86" s="73" t="s">
         <v>284</v>
@@ -8109,10 +8109,10 @@
         <v>292</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F87" s="73" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G87" s="69" t="s">
         <v>197</v>
@@ -8121,7 +8121,7 @@
         <v>134</v>
       </c>
       <c r="I87" s="63" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J87" s="41" t="s">
         <v>286</v>
@@ -8154,7 +8154,7 @@
         <v>301</v>
       </c>
       <c r="E88" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F88" s="75" t="s">
         <v>303</v>
@@ -8193,16 +8193,16 @@
         <v>299</v>
       </c>
       <c r="C89" s="84" t="s">
+        <v>653</v>
+      </c>
+      <c r="D89" s="69" t="s">
         <v>654</v>
       </c>
-      <c r="D89" s="69" t="s">
+      <c r="E89" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F89" s="73" t="s">
         <v>655</v>
-      </c>
-      <c r="E89" s="69" t="s">
-        <v>645</v>
-      </c>
-      <c r="F89" s="73" t="s">
-        <v>656</v>
       </c>
       <c r="G89" s="69" t="s">
         <v>227</v>
@@ -8211,7 +8211,7 @@
         <v>134</v>
       </c>
       <c r="I89" s="41" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J89" s="41" t="s">
         <v>286</v>
@@ -8244,10 +8244,10 @@
         <v>313</v>
       </c>
       <c r="E90" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F90" s="73" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G90" s="69" t="s">
         <v>243</v>
@@ -8289,10 +8289,10 @@
         <v>321</v>
       </c>
       <c r="E91" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F91" s="73" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G91" s="69" t="s">
         <v>197</v>
@@ -8334,10 +8334,10 @@
         <v>330</v>
       </c>
       <c r="E92" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F92" s="73" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G92" s="69" t="s">
         <v>197</v>
@@ -8379,10 +8379,10 @@
         <v>337</v>
       </c>
       <c r="E93" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F93" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F93" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G93" s="69" t="s">
         <v>243</v>
@@ -8424,10 +8424,10 @@
         <v>344</v>
       </c>
       <c r="E94" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F94" s="73" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G94" s="69" t="s">
         <v>227</v>
@@ -8469,10 +8469,10 @@
         <v>350</v>
       </c>
       <c r="E95" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F95" s="73" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G95" s="69" t="s">
         <v>227</v>
@@ -8514,10 +8514,10 @@
         <v>356</v>
       </c>
       <c r="E96" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F96" s="73" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G96" s="69" t="s">
         <v>197</v>
@@ -8559,10 +8559,10 @@
         <v>362</v>
       </c>
       <c r="E97" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F97" s="73" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G97" s="69" t="s">
         <v>197</v>
@@ -8604,10 +8604,10 @@
         <v>367</v>
       </c>
       <c r="E98" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F98" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F98" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G98" s="69" t="s">
         <v>243</v>
@@ -8643,16 +8643,16 @@
         <v>167</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E99" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F99" s="73" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G99" s="69" t="s">
         <v>118</v>
@@ -8661,7 +8661,7 @@
         <v>134</v>
       </c>
       <c r="I99" s="86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J99" s="38" t="s">
         <v>370</v>
@@ -8688,16 +8688,16 @@
         <v>167</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D100" s="69" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E100" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F100" s="73" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G100" s="69" t="s">
         <v>118</v>
@@ -8739,10 +8739,10 @@
         <v>381</v>
       </c>
       <c r="E101" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F101" s="73" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G101" s="69" t="s">
         <v>197</v>
@@ -8784,10 +8784,10 @@
         <v>539</v>
       </c>
       <c r="E102" s="69" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F102" s="73" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G102" s="69" t="s">
         <v>197</v>
@@ -8829,10 +8829,10 @@
         <v>387</v>
       </c>
       <c r="E103" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F103" s="73" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G103" s="69" t="s">
         <v>118</v>
@@ -8874,10 +8874,10 @@
         <v>387</v>
       </c>
       <c r="E104" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F104" s="73" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G104" s="69" t="s">
         <v>243</v>
@@ -8919,7 +8919,7 @@
         <v>394</v>
       </c>
       <c r="E105" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F105" s="73" t="s">
         <v>396</v>
@@ -8964,10 +8964,10 @@
         <v>401</v>
       </c>
       <c r="E106" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F106" s="73" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G106" s="69" t="s">
         <v>404</v>
@@ -9009,10 +9009,10 @@
         <v>401</v>
       </c>
       <c r="E107" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F107" s="73" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G107" s="69" t="s">
         <v>197</v>
@@ -9054,10 +9054,10 @@
         <v>414</v>
       </c>
       <c r="E108" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F108" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G108" s="69" t="s">
         <v>227</v>
@@ -9099,7 +9099,7 @@
         <v>420</v>
       </c>
       <c r="E109" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F109" s="73" t="s">
         <v>422</v>
@@ -9144,7 +9144,7 @@
         <v>426</v>
       </c>
       <c r="E110" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F110" s="73" t="s">
         <v>428</v>
@@ -9189,7 +9189,7 @@
         <v>433</v>
       </c>
       <c r="E111" s="85" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F111" s="73" t="s">
         <v>435</v>
@@ -9234,7 +9234,7 @@
         <v>439</v>
       </c>
       <c r="E112" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F112" s="73" t="s">
         <v>441</v>
@@ -9279,7 +9279,7 @@
         <v>444</v>
       </c>
       <c r="E113" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F113" s="73" t="s">
         <v>446</v>
@@ -9324,7 +9324,7 @@
         <v>449</v>
       </c>
       <c r="E114" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F114" s="73" t="s">
         <v>451</v>
@@ -9336,7 +9336,7 @@
         <v>134</v>
       </c>
       <c r="I114" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J114" s="41" t="s">
         <v>286</v>
@@ -9369,10 +9369,10 @@
         <v>454</v>
       </c>
       <c r="E115" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F115" s="73" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G115" s="69" t="s">
         <v>197</v>
@@ -9414,7 +9414,7 @@
         <v>458</v>
       </c>
       <c r="E116" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F116" s="73" t="s">
         <v>451</v>
@@ -9426,7 +9426,7 @@
         <v>134</v>
       </c>
       <c r="I116" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J116" s="41" t="s">
         <v>286</v>
@@ -9459,10 +9459,10 @@
         <v>462</v>
       </c>
       <c r="E117" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F117" s="73" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G117" s="69" t="s">
         <v>197</v>
@@ -9504,7 +9504,7 @@
         <v>552</v>
       </c>
       <c r="E118" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F118" s="73" t="s">
         <v>553</v>
@@ -9615,7 +9615,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C124" s="66" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D124" s="69" t="s">
         <v>477</v>
@@ -9816,22 +9816,22 @@
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B132" s="41" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C132" s="66" t="s">
         <v>499</v>
       </c>
       <c r="D132" s="79" t="s">
+        <v>688</v>
+      </c>
+      <c r="E132" s="38" t="s">
         <v>689</v>
       </c>
-      <c r="E132" s="38" t="s">
-        <v>690</v>
-      </c>
       <c r="F132" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="G132" s="38" t="s">
         <v>688</v>
-      </c>
-      <c r="G132" s="38" t="s">
-        <v>689</v>
       </c>
       <c r="H132" s="38"/>
       <c r="I132" s="38"/>
@@ -9839,7 +9839,7 @@
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C133" s="66" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D133" s="79" t="s">
         <v>476</v>
@@ -9859,7 +9859,7 @@
         <v>476</v>
       </c>
       <c r="E134" s="38" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F134" s="38"/>
       <c r="J134" s="54"/>
@@ -10064,7 +10064,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -10275,7 +10275,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C21" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D21" s="69" t="s">
         <v>55</v>
@@ -10287,7 +10287,7 @@
         <v>56</v>
       </c>
       <c r="G21" s="69" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H21" s="70" t="s">
         <v>58</v>
@@ -10298,7 +10298,7 @@
     </row>
     <row r="22" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C22" s="68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D22" s="69" t="s">
         <v>55</v>
@@ -10307,21 +10307,21 @@
         <v>54</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H22" s="70" t="s">
+        <v>576</v>
+      </c>
+      <c r="I22" s="69" t="s">
         <v>577</v>
-      </c>
-      <c r="I22" s="69" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C23" s="68" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D23" s="69" t="s">
         <v>55</v>
@@ -10330,22 +10330,22 @@
         <v>54</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="70" t="s">
+        <v>574</v>
+      </c>
+      <c r="I23" s="69" t="s">
         <v>575</v>
-      </c>
-      <c r="I23" s="69" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="59"/>
       <c r="C24" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>55</v>
@@ -10354,16 +10354,16 @@
         <v>54</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G24" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H24" s="70" t="s">
+        <v>614</v>
+      </c>
+      <c r="I24" s="69" t="s">
         <v>615</v>
-      </c>
-      <c r="I24" s="69" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -10437,19 +10437,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C28" s="68" t="s">
+        <v>579</v>
+      </c>
+      <c r="D28" s="69" t="s">
         <v>580</v>
       </c>
-      <c r="D28" s="69" t="s">
-        <v>581</v>
-      </c>
       <c r="E28" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H28" s="70" t="s">
         <v>140</v>
@@ -10463,10 +10463,10 @@
         <v>91</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E29" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F29" s="69" t="s">
         <v>93</v>
@@ -10483,22 +10483,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C30" s="68" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E30" s="69" t="s">
+        <v>596</v>
+      </c>
+      <c r="F30" s="69" t="s">
         <v>597</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>598</v>
       </c>
       <c r="G30" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H30" s="70" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I30" s="69" t="s">
         <v>501</v>
@@ -10506,141 +10506,141 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C31" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="D31" s="69" t="s">
         <v>590</v>
       </c>
-      <c r="D31" s="69" t="s">
-        <v>591</v>
-      </c>
       <c r="E31" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C32" s="68" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H32" s="70" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="33" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C33" s="68" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F33" s="69" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G33" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H33" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="I33" s="69" t="s">
         <v>610</v>
-      </c>
-      <c r="I33" s="69" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="34" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C34" s="68" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E34" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G34" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H34" s="70" t="s">
+        <v>616</v>
+      </c>
+      <c r="I34" s="69" t="s">
         <v>617</v>
-      </c>
-      <c r="I34" s="69" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="35" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C35" s="68" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E35" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G35" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H35" s="70" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I35" s="69" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K35"/>
     </row>
     <row r="36" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C36" s="68" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D36" s="69" t="s">
+        <v>595</v>
+      </c>
+      <c r="E36" s="69" t="s">
         <v>596</v>
       </c>
-      <c r="E36" s="69" t="s">
-        <v>597</v>
-      </c>
       <c r="F36" s="69" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G36" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H36" s="70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K36"/>
     </row>
@@ -10844,7 +10844,7 @@
         <v>148</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45" s="69" t="s">
         <v>149</v>
@@ -11184,7 +11184,7 @@
         <v>194</v>
       </c>
       <c r="E71" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F71" s="73" t="s">
         <v>196</v>
@@ -11223,16 +11223,16 @@
         <v>167</v>
       </c>
       <c r="C72" s="82" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D72" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E72" s="69" t="s">
+        <v>620</v>
+      </c>
+      <c r="F72" s="73" t="s">
         <v>621</v>
-      </c>
-      <c r="F72" s="73" t="s">
-        <v>622</v>
       </c>
       <c r="G72" s="69" t="s">
         <v>197</v>
@@ -11241,7 +11241,7 @@
         <v>134</v>
       </c>
       <c r="I72" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J72" t="s">
         <v>209</v>
@@ -11268,16 +11268,16 @@
         <v>167</v>
       </c>
       <c r="C73" s="82" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D73" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E73" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F73" s="73" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G73" s="69" t="s">
         <v>197</v>
@@ -11286,7 +11286,7 @@
         <v>134</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J73" s="41" t="s">
         <v>209</v>
@@ -11313,13 +11313,13 @@
         <v>167</v>
       </c>
       <c r="C74" s="82" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D74" s="69" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E74" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F74" s="73" t="s">
         <v>217</v>
@@ -11331,7 +11331,7 @@
         <v>134</v>
       </c>
       <c r="I74" s="63" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J74" t="s">
         <v>199</v>
@@ -11358,13 +11358,13 @@
         <v>167</v>
       </c>
       <c r="C75" s="82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D75" s="69" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E75" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F75" s="73" t="s">
         <v>217</v>
@@ -11376,7 +11376,7 @@
         <v>134</v>
       </c>
       <c r="I75" s="63" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J75" s="41" t="s">
         <v>199</v>
@@ -11403,16 +11403,16 @@
         <v>167</v>
       </c>
       <c r="C76" s="84" t="s">
+        <v>632</v>
+      </c>
+      <c r="D76" s="85" t="s">
         <v>633</v>
       </c>
-      <c r="D76" s="85" t="s">
-        <v>634</v>
-      </c>
       <c r="E76" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G76" s="74" t="s">
         <v>227</v>
@@ -11421,7 +11421,7 @@
         <v>134</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J76" s="40" t="s">
         <v>199</v>
@@ -11448,16 +11448,16 @@
         <v>167</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D77" s="85" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E77" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F77" s="77" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G77" s="74" t="s">
         <v>227</v>
@@ -11466,7 +11466,7 @@
         <v>134</v>
       </c>
       <c r="I77" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J77" s="40" t="s">
         <v>199</v>
@@ -11499,7 +11499,7 @@
         <v>233</v>
       </c>
       <c r="E78" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F78" s="75" t="s">
         <v>235</v>
@@ -11545,10 +11545,10 @@
         <v>240</v>
       </c>
       <c r="E79" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F79" s="73" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G79" s="69" t="s">
         <v>243</v>
@@ -11585,16 +11585,16 @@
         <v>167</v>
       </c>
       <c r="C80" s="84" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D80" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E80" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F80" s="73" t="s">
         <v>645</v>
-      </c>
-      <c r="F80" s="73" t="s">
-        <v>646</v>
       </c>
       <c r="G80" s="69" t="s">
         <v>129</v>
@@ -11630,16 +11630,16 @@
         <v>167</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D81" s="69" t="s">
+        <v>643</v>
+      </c>
+      <c r="E81" s="69" t="s">
         <v>644</v>
       </c>
-      <c r="E81" s="69" t="s">
-        <v>645</v>
-      </c>
       <c r="F81" s="73" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G81" s="69" t="s">
         <v>129</v>
@@ -11648,7 +11648,7 @@
         <v>134</v>
       </c>
       <c r="I81" s="41" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J81" s="41" t="s">
         <v>209</v>
@@ -11681,10 +11681,10 @@
         <v>256</v>
       </c>
       <c r="E82" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F82" s="77" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G82" s="85" t="s">
         <v>197</v>
@@ -11726,10 +11726,10 @@
         <v>263</v>
       </c>
       <c r="E83" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F83" s="77" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G83" s="85" t="s">
         <v>197</v>
@@ -11771,7 +11771,7 @@
         <v>268</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F84" s="73" t="s">
         <v>270</v>
@@ -11816,7 +11816,7 @@
         <v>277</v>
       </c>
       <c r="E85" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F85" s="73" t="s">
         <v>270</v>
@@ -11863,7 +11863,7 @@
         <v>282</v>
       </c>
       <c r="E86" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F86" s="73" t="s">
         <v>284</v>
@@ -11908,10 +11908,10 @@
         <v>292</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F87" s="73" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G87" s="69" t="s">
         <v>197</v>
@@ -11920,7 +11920,7 @@
         <v>134</v>
       </c>
       <c r="I87" s="63" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J87" t="s">
         <v>286</v>
@@ -11953,7 +11953,7 @@
         <v>301</v>
       </c>
       <c r="E88" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F88" s="75" t="s">
         <v>303</v>
@@ -11992,16 +11992,16 @@
         <v>299</v>
       </c>
       <c r="C89" s="84" t="s">
+        <v>653</v>
+      </c>
+      <c r="D89" s="69" t="s">
         <v>654</v>
       </c>
-      <c r="D89" s="69" t="s">
+      <c r="E89" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F89" s="73" t="s">
         <v>655</v>
-      </c>
-      <c r="E89" s="69" t="s">
-        <v>645</v>
-      </c>
-      <c r="F89" s="73" t="s">
-        <v>656</v>
       </c>
       <c r="G89" s="69" t="s">
         <v>227</v>
@@ -12010,7 +12010,7 @@
         <v>134</v>
       </c>
       <c r="I89" s="41" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J89" s="41" t="s">
         <v>286</v>
@@ -12043,10 +12043,10 @@
         <v>313</v>
       </c>
       <c r="E90" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F90" s="73" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G90" s="69" t="s">
         <v>243</v>
@@ -12088,10 +12088,10 @@
         <v>321</v>
       </c>
       <c r="E91" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F91" s="73" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G91" s="69" t="s">
         <v>197</v>
@@ -12133,10 +12133,10 @@
         <v>330</v>
       </c>
       <c r="E92" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F92" s="73" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G92" s="69" t="s">
         <v>197</v>
@@ -12178,10 +12178,10 @@
         <v>337</v>
       </c>
       <c r="E93" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F93" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F93" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G93" s="69" t="s">
         <v>243</v>
@@ -12223,10 +12223,10 @@
         <v>344</v>
       </c>
       <c r="E94" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F94" s="73" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G94" s="69" t="s">
         <v>227</v>
@@ -12268,10 +12268,10 @@
         <v>350</v>
       </c>
       <c r="E95" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F95" s="73" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G95" s="69" t="s">
         <v>227</v>
@@ -12313,10 +12313,10 @@
         <v>356</v>
       </c>
       <c r="E96" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F96" s="73" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G96" s="69" t="s">
         <v>197</v>
@@ -12358,10 +12358,10 @@
         <v>362</v>
       </c>
       <c r="E97" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F97" s="73" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G97" s="69" t="s">
         <v>197</v>
@@ -12403,10 +12403,10 @@
         <v>367</v>
       </c>
       <c r="E98" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F98" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F98" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G98" s="69" t="s">
         <v>243</v>
@@ -12442,16 +12442,16 @@
         <v>167</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E99" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F99" s="73" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G99" s="69" t="s">
         <v>118</v>
@@ -12460,7 +12460,7 @@
         <v>134</v>
       </c>
       <c r="I99" s="86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J99" s="38" t="s">
         <v>370</v>
@@ -12487,16 +12487,16 @@
         <v>167</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D100" s="69" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E100" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F100" s="73" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G100" s="69" t="s">
         <v>118</v>
@@ -12538,10 +12538,10 @@
         <v>381</v>
       </c>
       <c r="E101" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F101" s="73" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G101" s="69" t="s">
         <v>197</v>
@@ -12583,10 +12583,10 @@
         <v>539</v>
       </c>
       <c r="E102" s="69" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F102" s="73" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G102" s="69" t="s">
         <v>197</v>
@@ -12628,10 +12628,10 @@
         <v>387</v>
       </c>
       <c r="E103" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F103" s="73" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G103" s="69" t="s">
         <v>118</v>
@@ -12673,10 +12673,10 @@
         <v>387</v>
       </c>
       <c r="E104" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F104" s="73" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G104" s="69" t="s">
         <v>243</v>
@@ -12718,7 +12718,7 @@
         <v>394</v>
       </c>
       <c r="E105" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F105" s="73" t="s">
         <v>396</v>
@@ -12763,10 +12763,10 @@
         <v>401</v>
       </c>
       <c r="E106" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F106" s="73" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G106" s="69" t="s">
         <v>404</v>
@@ -12808,10 +12808,10 @@
         <v>401</v>
       </c>
       <c r="E107" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F107" s="73" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G107" s="69" t="s">
         <v>197</v>
@@ -12853,10 +12853,10 @@
         <v>414</v>
       </c>
       <c r="E108" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F108" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G108" s="69" t="s">
         <v>227</v>
@@ -12898,7 +12898,7 @@
         <v>420</v>
       </c>
       <c r="E109" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F109" s="73" t="s">
         <v>422</v>
@@ -12943,7 +12943,7 @@
         <v>426</v>
       </c>
       <c r="E110" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F110" s="73" t="s">
         <v>428</v>
@@ -12988,7 +12988,7 @@
         <v>433</v>
       </c>
       <c r="E111" s="85" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F111" s="73" t="s">
         <v>435</v>
@@ -13033,7 +13033,7 @@
         <v>439</v>
       </c>
       <c r="E112" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F112" s="73" t="s">
         <v>441</v>
@@ -13078,7 +13078,7 @@
         <v>444</v>
       </c>
       <c r="E113" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F113" s="73" t="s">
         <v>446</v>
@@ -13123,7 +13123,7 @@
         <v>449</v>
       </c>
       <c r="E114" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F114" s="73" t="s">
         <v>451</v>
@@ -13135,7 +13135,7 @@
         <v>134</v>
       </c>
       <c r="I114" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J114" t="s">
         <v>286</v>
@@ -13168,10 +13168,10 @@
         <v>454</v>
       </c>
       <c r="E115" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F115" s="73" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G115" s="69" t="s">
         <v>197</v>
@@ -13213,7 +13213,7 @@
         <v>458</v>
       </c>
       <c r="E116" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F116" s="73" t="s">
         <v>451</v>
@@ -13225,7 +13225,7 @@
         <v>134</v>
       </c>
       <c r="I116" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J116" t="s">
         <v>286</v>
@@ -13258,10 +13258,10 @@
         <v>462</v>
       </c>
       <c r="E117" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F117" s="73" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G117" s="69" t="s">
         <v>197</v>
@@ -13303,7 +13303,7 @@
         <v>552</v>
       </c>
       <c r="E118" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F118" s="73" t="s">
         <v>553</v>
@@ -13415,7 +13415,7 @@
     <row r="124" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A124" s="41"/>
       <c r="C124" s="66" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D124" s="69" t="s">
         <v>477</v>
@@ -13620,22 +13620,22 @@
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B132" s="41" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C132" s="66" t="s">
         <v>499</v>
       </c>
       <c r="D132" s="79" t="s">
+        <v>688</v>
+      </c>
+      <c r="E132" s="38" t="s">
         <v>689</v>
       </c>
-      <c r="E132" s="38" t="s">
-        <v>690</v>
-      </c>
       <c r="F132" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="G132" s="38" t="s">
         <v>688</v>
-      </c>
-      <c r="G132" s="38" t="s">
-        <v>689</v>
       </c>
       <c r="H132" s="38"/>
       <c r="I132" s="38"/>
@@ -13643,7 +13643,7 @@
     </row>
     <row r="133" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C133" s="66" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D133" s="79" t="s">
         <v>476</v>
@@ -13663,7 +13663,7 @@
         <v>476</v>
       </c>
       <c r="E134" s="38" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F134" s="38"/>
       <c r="J134" s="54"/>
@@ -13871,7 +13871,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -14082,7 +14082,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C21" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D21" s="69" t="s">
         <v>55</v>
@@ -14094,7 +14094,7 @@
         <v>56</v>
       </c>
       <c r="G21" s="69" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="H21" s="70" t="s">
         <v>58</v>
@@ -14105,7 +14105,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C22" s="68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D22" s="69" t="s">
         <v>55</v>
@@ -14114,21 +14114,21 @@
         <v>54</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H22" s="70" t="s">
+        <v>576</v>
+      </c>
+      <c r="I22" s="69" t="s">
         <v>577</v>
-      </c>
-      <c r="I22" s="69" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C23" s="68" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D23" s="69" t="s">
         <v>55</v>
@@ -14137,22 +14137,22 @@
         <v>54</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="70" t="s">
+        <v>574</v>
+      </c>
+      <c r="I23" s="69" t="s">
         <v>575</v>
-      </c>
-      <c r="I23" s="69" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="59"/>
       <c r="C24" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>55</v>
@@ -14161,16 +14161,16 @@
         <v>54</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G24" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H24" s="70" t="s">
+        <v>614</v>
+      </c>
+      <c r="I24" s="69" t="s">
         <v>615</v>
-      </c>
-      <c r="I24" s="69" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -14244,19 +14244,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C28" s="68" t="s">
+        <v>579</v>
+      </c>
+      <c r="D28" s="69" t="s">
         <v>580</v>
       </c>
-      <c r="D28" s="69" t="s">
-        <v>581</v>
-      </c>
       <c r="E28" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H28" s="70" t="s">
         <v>140</v>
@@ -14270,10 +14270,10 @@
         <v>91</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E29" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F29" s="69" t="s">
         <v>93</v>
@@ -14290,22 +14290,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C30" s="68" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E30" s="69" t="s">
+        <v>596</v>
+      </c>
+      <c r="F30" s="69" t="s">
         <v>597</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>598</v>
       </c>
       <c r="G30" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H30" s="70" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I30" s="69" t="s">
         <v>501</v>
@@ -14313,140 +14313,140 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C31" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="D31" s="69" t="s">
         <v>590</v>
       </c>
-      <c r="D31" s="69" t="s">
-        <v>591</v>
-      </c>
       <c r="E31" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C32" s="68" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H32" s="70" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C33" s="68" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F33" s="69" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G33" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H33" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="I33" s="69" t="s">
         <v>610</v>
-      </c>
-      <c r="I33" s="69" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C34" s="68" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E34" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G34" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H34" s="70" t="s">
+        <v>616</v>
+      </c>
+      <c r="I34" s="69" t="s">
         <v>617</v>
-      </c>
-      <c r="I34" s="69" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C35" s="68" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E35" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G35" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H35" s="70" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I35" s="69" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C36" s="68" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D36" s="69" t="s">
+        <v>595</v>
+      </c>
+      <c r="E36" s="69" t="s">
         <v>596</v>
       </c>
-      <c r="E36" s="69" t="s">
-        <v>597</v>
-      </c>
       <c r="F36" s="69" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G36" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H36" s="70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.45">
@@ -14641,7 +14641,7 @@
         <v>148</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45" s="69" t="s">
         <v>149</v>
@@ -14979,7 +14979,7 @@
         <v>194</v>
       </c>
       <c r="E71" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F71" s="73" t="s">
         <v>196</v>
@@ -15018,16 +15018,16 @@
         <v>167</v>
       </c>
       <c r="C72" s="82" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D72" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E72" s="69" t="s">
+        <v>620</v>
+      </c>
+      <c r="F72" s="73" t="s">
         <v>621</v>
-      </c>
-      <c r="F72" s="73" t="s">
-        <v>622</v>
       </c>
       <c r="G72" s="69" t="s">
         <v>197</v>
@@ -15036,7 +15036,7 @@
         <v>134</v>
       </c>
       <c r="I72" s="41" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J72" s="41" t="s">
         <v>209</v>
@@ -15063,16 +15063,16 @@
         <v>167</v>
       </c>
       <c r="C73" s="82" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D73" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E73" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F73" s="73" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G73" s="69" t="s">
         <v>197</v>
@@ -15081,7 +15081,7 @@
         <v>134</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J73" s="41" t="s">
         <v>209</v>
@@ -15108,13 +15108,13 @@
         <v>167</v>
       </c>
       <c r="C74" s="82" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D74" s="69" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E74" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F74" s="73" t="s">
         <v>217</v>
@@ -15126,7 +15126,7 @@
         <v>134</v>
       </c>
       <c r="I74" s="63" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J74" s="41" t="s">
         <v>199</v>
@@ -15153,13 +15153,13 @@
         <v>167</v>
       </c>
       <c r="C75" s="82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D75" s="69" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E75" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F75" s="73" t="s">
         <v>217</v>
@@ -15171,7 +15171,7 @@
         <v>134</v>
       </c>
       <c r="I75" s="63" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J75" s="41" t="s">
         <v>199</v>
@@ -15198,16 +15198,16 @@
         <v>167</v>
       </c>
       <c r="C76" s="84" t="s">
+        <v>632</v>
+      </c>
+      <c r="D76" s="85" t="s">
         <v>633</v>
       </c>
-      <c r="D76" s="85" t="s">
-        <v>634</v>
-      </c>
       <c r="E76" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G76" s="74" t="s">
         <v>227</v>
@@ -15216,7 +15216,7 @@
         <v>134</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J76" s="40" t="s">
         <v>199</v>
@@ -15243,16 +15243,16 @@
         <v>167</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D77" s="85" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E77" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F77" s="77" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G77" s="74" t="s">
         <v>227</v>
@@ -15261,7 +15261,7 @@
         <v>134</v>
       </c>
       <c r="I77" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J77" s="40" t="s">
         <v>199</v>
@@ -15294,7 +15294,7 @@
         <v>233</v>
       </c>
       <c r="E78" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F78" s="75" t="s">
         <v>235</v>
@@ -15339,10 +15339,10 @@
         <v>240</v>
       </c>
       <c r="E79" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F79" s="73" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G79" s="69" t="s">
         <v>243</v>
@@ -15378,16 +15378,16 @@
         <v>167</v>
       </c>
       <c r="C80" s="84" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D80" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E80" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F80" s="73" t="s">
         <v>645</v>
-      </c>
-      <c r="F80" s="73" t="s">
-        <v>646</v>
       </c>
       <c r="G80" s="69" t="s">
         <v>129</v>
@@ -15423,16 +15423,16 @@
         <v>167</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D81" s="69" t="s">
+        <v>643</v>
+      </c>
+      <c r="E81" s="69" t="s">
         <v>644</v>
       </c>
-      <c r="E81" s="69" t="s">
-        <v>645</v>
-      </c>
       <c r="F81" s="73" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G81" s="69" t="s">
         <v>129</v>
@@ -15441,7 +15441,7 @@
         <v>134</v>
       </c>
       <c r="I81" s="41" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J81" s="41" t="s">
         <v>209</v>
@@ -15474,10 +15474,10 @@
         <v>256</v>
       </c>
       <c r="E82" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F82" s="77" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G82" s="85" t="s">
         <v>197</v>
@@ -15519,10 +15519,10 @@
         <v>263</v>
       </c>
       <c r="E83" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F83" s="77" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G83" s="85" t="s">
         <v>197</v>
@@ -15564,7 +15564,7 @@
         <v>268</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F84" s="73" t="s">
         <v>270</v>
@@ -15609,7 +15609,7 @@
         <v>277</v>
       </c>
       <c r="E85" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F85" s="73" t="s">
         <v>270</v>
@@ -15656,7 +15656,7 @@
         <v>282</v>
       </c>
       <c r="E86" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F86" s="73" t="s">
         <v>284</v>
@@ -15701,10 +15701,10 @@
         <v>292</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F87" s="73" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G87" s="69" t="s">
         <v>197</v>
@@ -15713,7 +15713,7 @@
         <v>134</v>
       </c>
       <c r="I87" s="63" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J87" s="41" t="s">
         <v>286</v>
@@ -15746,7 +15746,7 @@
         <v>301</v>
       </c>
       <c r="E88" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F88" s="75" t="s">
         <v>303</v>
@@ -15785,16 +15785,16 @@
         <v>299</v>
       </c>
       <c r="C89" s="84" t="s">
+        <v>653</v>
+      </c>
+      <c r="D89" s="69" t="s">
         <v>654</v>
       </c>
-      <c r="D89" s="69" t="s">
+      <c r="E89" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F89" s="73" t="s">
         <v>655</v>
-      </c>
-      <c r="E89" s="69" t="s">
-        <v>645</v>
-      </c>
-      <c r="F89" s="73" t="s">
-        <v>656</v>
       </c>
       <c r="G89" s="69" t="s">
         <v>227</v>
@@ -15803,7 +15803,7 @@
         <v>134</v>
       </c>
       <c r="I89" s="41" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J89" s="41" t="s">
         <v>286</v>
@@ -15836,10 +15836,10 @@
         <v>313</v>
       </c>
       <c r="E90" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F90" s="73" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G90" s="69" t="s">
         <v>243</v>
@@ -15881,10 +15881,10 @@
         <v>321</v>
       </c>
       <c r="E91" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F91" s="73" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G91" s="69" t="s">
         <v>197</v>
@@ -15926,10 +15926,10 @@
         <v>330</v>
       </c>
       <c r="E92" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F92" s="73" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G92" s="69" t="s">
         <v>197</v>
@@ -15971,10 +15971,10 @@
         <v>337</v>
       </c>
       <c r="E93" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F93" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F93" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G93" s="69" t="s">
         <v>243</v>
@@ -16016,10 +16016,10 @@
         <v>344</v>
       </c>
       <c r="E94" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F94" s="73" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G94" s="69" t="s">
         <v>227</v>
@@ -16061,10 +16061,10 @@
         <v>350</v>
       </c>
       <c r="E95" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F95" s="73" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G95" s="69" t="s">
         <v>227</v>
@@ -16106,10 +16106,10 @@
         <v>356</v>
       </c>
       <c r="E96" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F96" s="73" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G96" s="69" t="s">
         <v>197</v>
@@ -16151,10 +16151,10 @@
         <v>362</v>
       </c>
       <c r="E97" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F97" s="73" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G97" s="69" t="s">
         <v>197</v>
@@ -16196,10 +16196,10 @@
         <v>367</v>
       </c>
       <c r="E98" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F98" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F98" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G98" s="69" t="s">
         <v>243</v>
@@ -16235,16 +16235,16 @@
         <v>167</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E99" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F99" s="73" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G99" s="69" t="s">
         <v>118</v>
@@ -16253,7 +16253,7 @@
         <v>134</v>
       </c>
       <c r="I99" s="86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J99" s="38" t="s">
         <v>370</v>
@@ -16280,16 +16280,16 @@
         <v>167</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D100" s="69" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E100" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F100" s="73" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G100" s="69" t="s">
         <v>118</v>
@@ -16331,10 +16331,10 @@
         <v>381</v>
       </c>
       <c r="E101" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F101" s="73" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G101" s="69" t="s">
         <v>197</v>
@@ -16376,10 +16376,10 @@
         <v>539</v>
       </c>
       <c r="E102" s="69" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F102" s="73" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G102" s="69" t="s">
         <v>197</v>
@@ -16421,10 +16421,10 @@
         <v>387</v>
       </c>
       <c r="E103" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F103" s="73" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G103" s="69" t="s">
         <v>118</v>
@@ -16466,10 +16466,10 @@
         <v>387</v>
       </c>
       <c r="E104" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F104" s="73" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G104" s="69" t="s">
         <v>243</v>
@@ -16511,7 +16511,7 @@
         <v>394</v>
       </c>
       <c r="E105" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F105" s="73" t="s">
         <v>396</v>
@@ -16556,10 +16556,10 @@
         <v>401</v>
       </c>
       <c r="E106" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F106" s="73" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G106" s="69" t="s">
         <v>404</v>
@@ -16601,10 +16601,10 @@
         <v>401</v>
       </c>
       <c r="E107" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F107" s="73" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G107" s="69" t="s">
         <v>197</v>
@@ -16646,10 +16646,10 @@
         <v>414</v>
       </c>
       <c r="E108" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F108" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G108" s="69" t="s">
         <v>227</v>
@@ -16691,7 +16691,7 @@
         <v>420</v>
       </c>
       <c r="E109" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F109" s="73" t="s">
         <v>422</v>
@@ -16736,7 +16736,7 @@
         <v>426</v>
       </c>
       <c r="E110" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F110" s="73" t="s">
         <v>428</v>
@@ -16781,7 +16781,7 @@
         <v>433</v>
       </c>
       <c r="E111" s="85" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F111" s="73" t="s">
         <v>435</v>
@@ -16826,7 +16826,7 @@
         <v>439</v>
       </c>
       <c r="E112" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F112" s="73" t="s">
         <v>441</v>
@@ -16871,7 +16871,7 @@
         <v>444</v>
       </c>
       <c r="E113" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F113" s="73" t="s">
         <v>446</v>
@@ -16916,7 +16916,7 @@
         <v>449</v>
       </c>
       <c r="E114" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F114" s="73" t="s">
         <v>451</v>
@@ -16928,7 +16928,7 @@
         <v>134</v>
       </c>
       <c r="I114" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J114" s="41" t="s">
         <v>286</v>
@@ -16961,10 +16961,10 @@
         <v>454</v>
       </c>
       <c r="E115" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F115" s="73" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G115" s="69" t="s">
         <v>197</v>
@@ -17006,7 +17006,7 @@
         <v>458</v>
       </c>
       <c r="E116" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F116" s="73" t="s">
         <v>451</v>
@@ -17018,7 +17018,7 @@
         <v>134</v>
       </c>
       <c r="I116" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J116" s="41" t="s">
         <v>286</v>
@@ -17051,10 +17051,10 @@
         <v>462</v>
       </c>
       <c r="E117" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F117" s="73" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G117" s="69" t="s">
         <v>197</v>
@@ -17096,7 +17096,7 @@
         <v>552</v>
       </c>
       <c r="E118" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F118" s="73" t="s">
         <v>553</v>
@@ -17207,7 +17207,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C124" s="66" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D124" s="69" t="s">
         <v>477</v>
@@ -17408,22 +17408,22 @@
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B132" s="41" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C132" s="66" t="s">
         <v>499</v>
       </c>
       <c r="D132" s="79" t="s">
+        <v>688</v>
+      </c>
+      <c r="E132" s="38" t="s">
         <v>689</v>
       </c>
-      <c r="E132" s="38" t="s">
-        <v>690</v>
-      </c>
       <c r="F132" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="G132" s="38" t="s">
         <v>688</v>
-      </c>
-      <c r="G132" s="38" t="s">
-        <v>689</v>
       </c>
       <c r="H132" s="38"/>
       <c r="I132" s="38"/>
@@ -17431,7 +17431,7 @@
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C133" s="66" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D133" s="79" t="s">
         <v>476</v>
@@ -17451,7 +17451,7 @@
         <v>476</v>
       </c>
       <c r="E134" s="38" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F134" s="38"/>
       <c r="J134" s="54"/>
@@ -17600,7 +17600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+    <sheetView topLeftCell="C19" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -17658,7 +17658,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -17869,7 +17869,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C21" s="68" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D21" s="69" t="s">
         <v>55</v>
@@ -17881,7 +17881,7 @@
         <v>56</v>
       </c>
       <c r="G21" s="69" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="H21" s="70" t="s">
         <v>58</v>
@@ -17892,7 +17892,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C22" s="68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D22" s="69" t="s">
         <v>55</v>
@@ -17901,21 +17901,21 @@
         <v>54</v>
       </c>
       <c r="F22" s="69" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H22" s="70" t="s">
+        <v>576</v>
+      </c>
+      <c r="I22" s="69" t="s">
         <v>577</v>
-      </c>
-      <c r="I22" s="69" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C23" s="68" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D23" s="69" t="s">
         <v>55</v>
@@ -17924,22 +17924,22 @@
         <v>54</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="70" t="s">
+        <v>574</v>
+      </c>
+      <c r="I23" s="69" t="s">
         <v>575</v>
-      </c>
-      <c r="I23" s="69" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="59"/>
       <c r="C24" s="68" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D24" s="69" t="s">
         <v>55</v>
@@ -17948,16 +17948,16 @@
         <v>54</v>
       </c>
       <c r="F24" s="69" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G24" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H24" s="70" t="s">
+        <v>614</v>
+      </c>
+      <c r="I24" s="69" t="s">
         <v>615</v>
-      </c>
-      <c r="I24" s="69" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -18031,19 +18031,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C28" s="68" t="s">
+        <v>579</v>
+      </c>
+      <c r="D28" s="69" t="s">
         <v>580</v>
       </c>
-      <c r="D28" s="69" t="s">
-        <v>581</v>
-      </c>
       <c r="E28" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F28" s="69" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G28" s="69" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H28" s="70" t="s">
         <v>140</v>
@@ -18057,10 +18057,10 @@
         <v>91</v>
       </c>
       <c r="D29" s="69" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E29" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F29" s="69" t="s">
         <v>93</v>
@@ -18077,22 +18077,22 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C30" s="68" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D30" s="69" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E30" s="69" t="s">
+        <v>596</v>
+      </c>
+      <c r="F30" s="69" t="s">
         <v>597</v>
-      </c>
-      <c r="F30" s="69" t="s">
-        <v>598</v>
       </c>
       <c r="G30" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H30" s="70" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I30" s="69" t="s">
         <v>501</v>
@@ -18100,140 +18100,140 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C31" s="68" t="s">
+        <v>589</v>
+      </c>
+      <c r="D31" s="69" t="s">
         <v>590</v>
       </c>
-      <c r="D31" s="69" t="s">
-        <v>591</v>
-      </c>
       <c r="E31" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F31" s="69" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I31" s="69" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C32" s="68" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D32" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F32" s="69" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G32" s="69" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H32" s="70" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I32" s="69" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C33" s="68" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D33" s="69" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E33" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F33" s="69" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G33" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H33" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="I33" s="69" t="s">
         <v>610</v>
-      </c>
-      <c r="I33" s="69" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C34" s="68" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E34" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F34" s="69" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G34" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H34" s="70" t="s">
+        <v>616</v>
+      </c>
+      <c r="I34" s="69" t="s">
         <v>617</v>
-      </c>
-      <c r="I34" s="69" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C35" s="68" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D35" s="69" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E35" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F35" s="69" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G35" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H35" s="70" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I35" s="69" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C36" s="68" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D36" s="69" t="s">
+        <v>595</v>
+      </c>
+      <c r="E36" s="69" t="s">
         <v>596</v>
       </c>
-      <c r="E36" s="69" t="s">
-        <v>597</v>
-      </c>
       <c r="F36" s="69" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="G36" s="69" t="s">
         <v>51</v>
       </c>
       <c r="H36" s="70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.45">
@@ -18428,7 +18428,7 @@
         <v>148</v>
       </c>
       <c r="E45" s="69" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F45" s="69" t="s">
         <v>149</v>
@@ -18766,7 +18766,7 @@
         <v>194</v>
       </c>
       <c r="E71" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F71" s="73" t="s">
         <v>196</v>
@@ -18805,16 +18805,16 @@
         <v>167</v>
       </c>
       <c r="C72" s="82" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D72" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E72" s="69" t="s">
+        <v>620</v>
+      </c>
+      <c r="F72" s="73" t="s">
         <v>621</v>
-      </c>
-      <c r="F72" s="73" t="s">
-        <v>622</v>
       </c>
       <c r="G72" s="69" t="s">
         <v>197</v>
@@ -18823,7 +18823,7 @@
         <v>134</v>
       </c>
       <c r="I72" s="41" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="J72" s="41" t="s">
         <v>209</v>
@@ -18850,16 +18850,16 @@
         <v>167</v>
       </c>
       <c r="C73" s="82" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D73" s="69" t="s">
         <v>205</v>
       </c>
       <c r="E73" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F73" s="73" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="G73" s="69" t="s">
         <v>197</v>
@@ -18868,7 +18868,7 @@
         <v>134</v>
       </c>
       <c r="I73" s="41" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J73" s="41" t="s">
         <v>209</v>
@@ -18895,13 +18895,13 @@
         <v>167</v>
       </c>
       <c r="C74" s="82" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D74" s="69" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E74" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F74" s="73" t="s">
         <v>217</v>
@@ -18913,7 +18913,7 @@
         <v>134</v>
       </c>
       <c r="I74" s="63" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="J74" s="41" t="s">
         <v>199</v>
@@ -18940,13 +18940,13 @@
         <v>167</v>
       </c>
       <c r="C75" s="82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D75" s="69" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E75" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F75" s="73" t="s">
         <v>217</v>
@@ -18958,7 +18958,7 @@
         <v>134</v>
       </c>
       <c r="I75" s="63" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="J75" s="41" t="s">
         <v>199</v>
@@ -18985,16 +18985,16 @@
         <v>167</v>
       </c>
       <c r="C76" s="84" t="s">
+        <v>632</v>
+      </c>
+      <c r="D76" s="85" t="s">
         <v>633</v>
       </c>
-      <c r="D76" s="85" t="s">
-        <v>634</v>
-      </c>
       <c r="E76" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F76" s="77" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="G76" s="74" t="s">
         <v>227</v>
@@ -19003,7 +19003,7 @@
         <v>134</v>
       </c>
       <c r="I76" s="40" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="J76" s="40" t="s">
         <v>199</v>
@@ -19030,16 +19030,16 @@
         <v>167</v>
       </c>
       <c r="C77" s="84" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D77" s="85" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E77" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F77" s="77" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G77" s="74" t="s">
         <v>227</v>
@@ -19048,7 +19048,7 @@
         <v>134</v>
       </c>
       <c r="I77" s="41" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J77" s="40" t="s">
         <v>199</v>
@@ -19081,7 +19081,7 @@
         <v>233</v>
       </c>
       <c r="E78" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F78" s="75" t="s">
         <v>235</v>
@@ -19126,10 +19126,10 @@
         <v>240</v>
       </c>
       <c r="E79" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F79" s="73" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G79" s="69" t="s">
         <v>243</v>
@@ -19165,16 +19165,16 @@
         <v>167</v>
       </c>
       <c r="C80" s="84" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D80" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E80" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F80" s="73" t="s">
         <v>645</v>
-      </c>
-      <c r="F80" s="73" t="s">
-        <v>646</v>
       </c>
       <c r="G80" s="69" t="s">
         <v>129</v>
@@ -19210,16 +19210,16 @@
         <v>167</v>
       </c>
       <c r="C81" s="84" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D81" s="69" t="s">
+        <v>643</v>
+      </c>
+      <c r="E81" s="69" t="s">
         <v>644</v>
       </c>
-      <c r="E81" s="69" t="s">
-        <v>645</v>
-      </c>
       <c r="F81" s="73" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G81" s="69" t="s">
         <v>129</v>
@@ -19228,7 +19228,7 @@
         <v>134</v>
       </c>
       <c r="I81" s="41" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="J81" s="41" t="s">
         <v>209</v>
@@ -19261,10 +19261,10 @@
         <v>256</v>
       </c>
       <c r="E82" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F82" s="77" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G82" s="85" t="s">
         <v>197</v>
@@ -19306,10 +19306,10 @@
         <v>263</v>
       </c>
       <c r="E83" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F83" s="77" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G83" s="85" t="s">
         <v>197</v>
@@ -19351,7 +19351,7 @@
         <v>268</v>
       </c>
       <c r="E84" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F84" s="73" t="s">
         <v>270</v>
@@ -19396,7 +19396,7 @@
         <v>277</v>
       </c>
       <c r="E85" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F85" s="73" t="s">
         <v>270</v>
@@ -19443,7 +19443,7 @@
         <v>282</v>
       </c>
       <c r="E86" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F86" s="73" t="s">
         <v>284</v>
@@ -19488,10 +19488,10 @@
         <v>292</v>
       </c>
       <c r="E87" s="69" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="F87" s="73" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G87" s="69" t="s">
         <v>197</v>
@@ -19500,7 +19500,7 @@
         <v>134</v>
       </c>
       <c r="I87" s="63" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J87" s="41" t="s">
         <v>286</v>
@@ -19533,7 +19533,7 @@
         <v>301</v>
       </c>
       <c r="E88" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F88" s="75" t="s">
         <v>303</v>
@@ -19572,16 +19572,16 @@
         <v>299</v>
       </c>
       <c r="C89" s="84" t="s">
+        <v>653</v>
+      </c>
+      <c r="D89" s="69" t="s">
         <v>654</v>
       </c>
-      <c r="D89" s="69" t="s">
+      <c r="E89" s="69" t="s">
+        <v>644</v>
+      </c>
+      <c r="F89" s="73" t="s">
         <v>655</v>
-      </c>
-      <c r="E89" s="69" t="s">
-        <v>645</v>
-      </c>
-      <c r="F89" s="73" t="s">
-        <v>656</v>
       </c>
       <c r="G89" s="69" t="s">
         <v>227</v>
@@ -19590,7 +19590,7 @@
         <v>134</v>
       </c>
       <c r="I89" s="41" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J89" s="41" t="s">
         <v>286</v>
@@ -19623,10 +19623,10 @@
         <v>313</v>
       </c>
       <c r="E90" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F90" s="73" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G90" s="69" t="s">
         <v>243</v>
@@ -19668,10 +19668,10 @@
         <v>321</v>
       </c>
       <c r="E91" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F91" s="73" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G91" s="69" t="s">
         <v>197</v>
@@ -19713,10 +19713,10 @@
         <v>330</v>
       </c>
       <c r="E92" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F92" s="73" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G92" s="69" t="s">
         <v>197</v>
@@ -19758,10 +19758,10 @@
         <v>337</v>
       </c>
       <c r="E93" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F93" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F93" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G93" s="69" t="s">
         <v>243</v>
@@ -19803,10 +19803,10 @@
         <v>344</v>
       </c>
       <c r="E94" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F94" s="73" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G94" s="69" t="s">
         <v>227</v>
@@ -19848,10 +19848,10 @@
         <v>350</v>
       </c>
       <c r="E95" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F95" s="73" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G95" s="69" t="s">
         <v>227</v>
@@ -19893,10 +19893,10 @@
         <v>356</v>
       </c>
       <c r="E96" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F96" s="73" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G96" s="69" t="s">
         <v>197</v>
@@ -19938,10 +19938,10 @@
         <v>362</v>
       </c>
       <c r="E97" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F97" s="73" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G97" s="69" t="s">
         <v>197</v>
@@ -19983,10 +19983,10 @@
         <v>367</v>
       </c>
       <c r="E98" s="69" t="s">
+        <v>618</v>
+      </c>
+      <c r="F98" s="73" t="s">
         <v>619</v>
-      </c>
-      <c r="F98" s="73" t="s">
-        <v>620</v>
       </c>
       <c r="G98" s="69" t="s">
         <v>243</v>
@@ -20022,16 +20022,16 @@
         <v>167</v>
       </c>
       <c r="C99" s="84" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D99" s="69" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E99" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F99" s="73" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G99" s="69" t="s">
         <v>118</v>
@@ -20040,7 +20040,7 @@
         <v>134</v>
       </c>
       <c r="I99" s="86" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="J99" s="38" t="s">
         <v>370</v>
@@ -20067,16 +20067,16 @@
         <v>167</v>
       </c>
       <c r="C100" s="84" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D100" s="69" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E100" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F100" s="73" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G100" s="69" t="s">
         <v>118</v>
@@ -20118,10 +20118,10 @@
         <v>381</v>
       </c>
       <c r="E101" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F101" s="73" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G101" s="69" t="s">
         <v>197</v>
@@ -20163,10 +20163,10 @@
         <v>539</v>
       </c>
       <c r="E102" s="69" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F102" s="73" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G102" s="69" t="s">
         <v>197</v>
@@ -20208,10 +20208,10 @@
         <v>387</v>
       </c>
       <c r="E103" s="69" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F103" s="73" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G103" s="69" t="s">
         <v>118</v>
@@ -20253,10 +20253,10 @@
         <v>387</v>
       </c>
       <c r="E104" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F104" s="73" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G104" s="69" t="s">
         <v>243</v>
@@ -20298,7 +20298,7 @@
         <v>394</v>
       </c>
       <c r="E105" s="69" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F105" s="73" t="s">
         <v>396</v>
@@ -20343,10 +20343,10 @@
         <v>401</v>
       </c>
       <c r="E106" s="69" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F106" s="73" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G106" s="69" t="s">
         <v>404</v>
@@ -20388,10 +20388,10 @@
         <v>401</v>
       </c>
       <c r="E107" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F107" s="73" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G107" s="69" t="s">
         <v>197</v>
@@ -20433,10 +20433,10 @@
         <v>414</v>
       </c>
       <c r="E108" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F108" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G108" s="69" t="s">
         <v>227</v>
@@ -20478,7 +20478,7 @@
         <v>420</v>
       </c>
       <c r="E109" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F109" s="73" t="s">
         <v>422</v>
@@ -20523,7 +20523,7 @@
         <v>426</v>
       </c>
       <c r="E110" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F110" s="73" t="s">
         <v>428</v>
@@ -20568,7 +20568,7 @@
         <v>433</v>
       </c>
       <c r="E111" s="85" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F111" s="73" t="s">
         <v>435</v>
@@ -20613,7 +20613,7 @@
         <v>439</v>
       </c>
       <c r="E112" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F112" s="73" t="s">
         <v>441</v>
@@ -20658,7 +20658,7 @@
         <v>444</v>
       </c>
       <c r="E113" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F113" s="73" t="s">
         <v>446</v>
@@ -20703,7 +20703,7 @@
         <v>449</v>
       </c>
       <c r="E114" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F114" s="73" t="s">
         <v>451</v>
@@ -20715,7 +20715,7 @@
         <v>134</v>
       </c>
       <c r="I114" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J114" s="41" t="s">
         <v>286</v>
@@ -20748,10 +20748,10 @@
         <v>454</v>
       </c>
       <c r="E115" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F115" s="73" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G115" s="69" t="s">
         <v>197</v>
@@ -20793,7 +20793,7 @@
         <v>458</v>
       </c>
       <c r="E116" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F116" s="73" t="s">
         <v>451</v>
@@ -20805,7 +20805,7 @@
         <v>134</v>
       </c>
       <c r="I116" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J116" s="41" t="s">
         <v>286</v>
@@ -20838,10 +20838,10 @@
         <v>462</v>
       </c>
       <c r="E117" s="85" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F117" s="73" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G117" s="69" t="s">
         <v>197</v>
@@ -20883,7 +20883,7 @@
         <v>552</v>
       </c>
       <c r="E118" s="85" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F118" s="73" t="s">
         <v>553</v>
@@ -20994,7 +20994,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C124" s="66" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D124" s="69" t="s">
         <v>477</v>
@@ -21195,22 +21195,22 @@
     </row>
     <row r="132" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B132" s="41" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C132" s="66" t="s">
         <v>499</v>
       </c>
       <c r="D132" s="79" t="s">
+        <v>688</v>
+      </c>
+      <c r="E132" s="38" t="s">
         <v>689</v>
       </c>
-      <c r="E132" s="38" t="s">
-        <v>690</v>
-      </c>
       <c r="F132" s="38" t="s">
+        <v>687</v>
+      </c>
+      <c r="G132" s="38" t="s">
         <v>688</v>
-      </c>
-      <c r="G132" s="38" t="s">
-        <v>689</v>
       </c>
       <c r="H132" s="38"/>
       <c r="I132" s="38"/>
@@ -21218,7 +21218,7 @@
     </row>
     <row r="133" spans="2:11" x14ac:dyDescent="0.45">
       <c r="C133" s="66" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D133" s="79" t="s">
         <v>476</v>
@@ -21238,7 +21238,7 @@
         <v>476</v>
       </c>
       <c r="E134" s="38" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="F134" s="38"/>
       <c r="J134" s="54"/>

</xml_diff>

<commit_message>
Version running for the Aug 16 report.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_0.xlsx
+++ b/RECC_Config_V2_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="10" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="1" state="visible" r:id="rId1"/>
@@ -804,7 +804,7 @@
       <c r="C4" s="1" t="n"/>
       <c r="D4" s="77" t="inlineStr">
         <is>
-          <t>RECC_Germany</t>
+          <t>RECC_R32CHN</t>
         </is>
       </c>
       <c r="G4" s="27" t="n"/>
@@ -948,8 +948,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -967,8 +967,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -7341,8 +7341,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -7360,8 +7360,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -9384,7 +9384,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -12511,7 +12511,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -13734,8 +13734,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -13753,8 +13753,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -15777,7 +15777,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -18904,7 +18904,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -20127,8 +20127,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -20146,8 +20146,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -22170,7 +22170,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -25297,7 +25297,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -26209,7 +26209,7 @@
       </c>
       <c r="D142" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E142" s="37" t="inlineStr">
@@ -26237,7 +26237,7 @@
       </c>
       <c r="D143" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E143" s="37" t="inlineStr">
@@ -26265,7 +26265,7 @@
       </c>
       <c r="D144" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E144" s="37" t="inlineStr">
@@ -26320,7 +26320,7 @@
       </c>
       <c r="D146" s="75" t="inlineStr">
         <is>
-          <t>['pav']</t>
+          <t>['reb']</t>
         </is>
       </c>
       <c r="E146" s="37" t="inlineStr">
@@ -31422,8 +31422,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="C70" workbookViewId="0">
+      <selection activeCell="I127" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -31441,8 +31441,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -33465,7 +33465,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -36592,7 +36592,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -37181,7 +37181,7 @@
       </c>
       <c r="D132" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -37216,7 +37216,7 @@
       </c>
       <c r="D133" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -37251,7 +37251,7 @@
       </c>
       <c r="D134" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E134" s="37" t="inlineStr">
@@ -37284,7 +37284,7 @@
       </c>
       <c r="D135" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -37313,7 +37313,7 @@
       </c>
       <c r="D136" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -37342,7 +37342,7 @@
       </c>
       <c r="D137" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E137" s="37" t="inlineStr">
@@ -37371,7 +37371,7 @@
       </c>
       <c r="D138" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -37403,7 +37403,7 @@
       </c>
       <c r="D139" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -37435,7 +37435,7 @@
       </c>
       <c r="D140" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E140" s="37" t="inlineStr">
@@ -37467,7 +37467,7 @@
       </c>
       <c r="D141" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E141" s="37" t="inlineStr">
@@ -37532,7 +37532,7 @@
       </c>
       <c r="D143" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E143" s="37" t="inlineStr">
@@ -37560,7 +37560,7 @@
       </c>
       <c r="D144" s="82" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E144" s="37" t="inlineStr">
@@ -37815,8 +37815,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A67" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -37834,8 +37834,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -39858,7 +39858,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -42985,7 +42985,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -43764,7 +43764,7 @@
       </c>
       <c r="D138" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -43796,7 +43796,7 @@
       </c>
       <c r="D139" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -43828,7 +43828,7 @@
       </c>
       <c r="D140" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E140" s="37" t="inlineStr">
@@ -43860,7 +43860,7 @@
       </c>
       <c r="D141" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E141" s="37" t="inlineStr">
@@ -43925,7 +43925,7 @@
       </c>
       <c r="D143" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E143" s="37" t="inlineStr">
@@ -43953,7 +43953,7 @@
       </c>
       <c r="D144" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E144" s="37" t="inlineStr">
@@ -44208,8 +44208,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -44227,8 +44227,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -46251,7 +46251,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -49378,7 +49378,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -50601,8 +50601,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="B34" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -50620,8 +50620,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -52644,7 +52644,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -55771,7 +55771,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -56360,7 +56360,7 @@
       </c>
       <c r="D132" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -56395,7 +56395,7 @@
       </c>
       <c r="D133" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -56430,7 +56430,7 @@
       </c>
       <c r="D134" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E134" s="37" t="inlineStr">
@@ -56463,7 +56463,7 @@
       </c>
       <c r="D135" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -56492,7 +56492,7 @@
       </c>
       <c r="D136" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -56521,7 +56521,7 @@
       </c>
       <c r="D137" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E137" s="37" t="inlineStr">
@@ -56550,7 +56550,7 @@
       </c>
       <c r="D138" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -56582,7 +56582,7 @@
       </c>
       <c r="D139" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -56614,7 +56614,7 @@
       </c>
       <c r="D140" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E140" s="37" t="inlineStr">
@@ -56646,7 +56646,7 @@
       </c>
       <c r="D141" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E141" s="37" t="inlineStr">
@@ -56711,7 +56711,7 @@
       </c>
       <c r="D143" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E143" s="37" t="inlineStr">
@@ -56739,7 +56739,7 @@
       </c>
       <c r="D144" s="82" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E144" s="37" t="inlineStr">
@@ -56995,8 +56995,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -57014,8 +57014,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -59038,7 +59038,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -62165,7 +62165,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -63388,8 +63388,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="E61" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -63407,8 +63407,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -65431,7 +65431,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -68558,7 +68558,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">
@@ -69781,8 +69781,8 @@
   </sheetPr>
   <dimension ref="A2:Q163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -69800,8 +69800,8 @@
     <col customWidth="1" max="12" min="12" style="80" width="73.53125"/>
     <col customWidth="1" max="13" min="13" style="80" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="80" width="90"/>
-    <col customWidth="1" max="27" min="15" style="80" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="28" style="80" width="10.6640625"/>
+    <col customWidth="1" max="29" min="15" style="80" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="30" style="80" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -71824,7 +71824,7 @@
       </c>
       <c r="I75" s="60" t="inlineStr">
         <is>
-          <t>735e41ad-cd3f-4e92-a414-af7af2a83a64</t>
+          <t>9a247cb1-aa78-45f7-ba51-d4c4e7dbef52</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
@@ -74951,7 +74951,7 @@
       </c>
       <c r="I120" s="60" t="inlineStr">
         <is>
-          <t>7f68bf46-3e70-4bb6-ab16-5b5a4417302f</t>
+          <t>dafb9643-a1d9-4c03-b1e7-1a66f8ef7459</t>
         </is>
       </c>
       <c r="J120" t="inlineStr">

</xml_diff>